<commit_message>
Tiedoston pienentäminen videon kuvausta varten
</commit_message>
<xml_diff>
--- a/Input data/Lappeenrannan kaupungin ostolaskut 2020_testiversio.xlsx
+++ b/Input data/Lappeenrannan kaupungin ostolaskut 2020_testiversio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jere\Documents\UiPath\netvisorRobo\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C5BA72-52CB-4802-9DEB-EFAC9C7B712D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516035D5-12CB-4F4C-A777-77886F37769B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="3690" windowWidth="28785" windowHeight="16335" xr2:uid="{EAE8BAAB-E8FA-4BAC-ACC3-9B83FB8CA550}"/>
+    <workbookView xWindow="7335" yWindow="2250" windowWidth="30675" windowHeight="16335" xr2:uid="{EAE8BAAB-E8FA-4BAC-ACC3-9B83FB8CA550}"/>
   </bookViews>
   <sheets>
     <sheet name="Ostolaskudata 2020" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
   <si>
     <t>Kuntanro</t>
   </si>
@@ -518,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF957FA-1780-4970-93E2-B725464F5534}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +532,8 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -657,6 +659,9 @@
       <c r="E3">
         <v>20908</v>
       </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
@@ -861,7 +866,7 @@
         <v>44133</v>
       </c>
       <c r="D7">
-        <v>4860</v>
+        <v>5474</v>
       </c>
       <c r="E7">
         <v>34912</v>
@@ -885,7 +890,7 @@
         <v>36</v>
       </c>
       <c r="L7">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M7">
         <v>30</v>
@@ -914,7 +919,7 @@
         <v>44133</v>
       </c>
       <c r="D8">
-        <v>4932</v>
+        <v>5566</v>
       </c>
       <c r="E8">
         <v>34912</v>
@@ -938,7 +943,7 @@
         <v>36</v>
       </c>
       <c r="L8">
-        <v>11419.94</v>
+        <v>31142.04</v>
       </c>
       <c r="M8">
         <v>30</v>
@@ -953,7 +958,7 @@
         <v>29</v>
       </c>
       <c r="Q8">
-        <v>3400</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -967,7 +972,7 @@
         <v>44133</v>
       </c>
       <c r="D9">
-        <v>5474</v>
+        <v>5566</v>
       </c>
       <c r="E9">
         <v>34912</v>
@@ -991,7 +996,7 @@
         <v>36</v>
       </c>
       <c r="L9">
-        <v>300967.34999999998</v>
+        <v>33</v>
       </c>
       <c r="M9">
         <v>30</v>
@@ -1006,7 +1011,7 @@
         <v>29</v>
       </c>
       <c r="Q9">
-        <v>3402</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1017,46 +1022,49 @@
         <v>17</v>
       </c>
       <c r="C10" s="3">
-        <v>44133</v>
+        <v>44121</v>
       </c>
       <c r="D10">
-        <v>5474</v>
+        <v>4209</v>
       </c>
       <c r="E10">
-        <v>34912</v>
+        <v>1670</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H10">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J10">
-        <v>4420</v>
+        <v>4580</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="L10">
+        <v>21</v>
       </c>
       <c r="M10">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="N10" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="O10">
-        <v>340</v>
+        <v>420</v>
       </c>
       <c r="P10" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="Q10">
-        <v>3400</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1067,49 +1075,49 @@
         <v>17</v>
       </c>
       <c r="C11" s="3">
-        <v>44133</v>
+        <v>44121</v>
       </c>
       <c r="D11">
-        <v>5566</v>
+        <v>4209</v>
       </c>
       <c r="E11">
-        <v>34912</v>
+        <v>1670</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H11">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J11">
-        <v>4420</v>
+        <v>4580</v>
       </c>
       <c r="K11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L11">
-        <v>31142.04</v>
+        <v>222</v>
       </c>
       <c r="M11">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="N11" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="O11">
-        <v>340</v>
+        <v>420</v>
       </c>
       <c r="P11" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="Q11">
-        <v>3401</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1120,19 +1128,19 @@
         <v>17</v>
       </c>
       <c r="C12" s="3">
-        <v>44133</v>
+        <v>44105</v>
       </c>
       <c r="D12">
-        <v>5566</v>
+        <v>2673</v>
       </c>
       <c r="E12">
-        <v>34912</v>
+        <v>20908</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H12">
         <v>43</v>
@@ -1141,13 +1149,13 @@
         <v>26</v>
       </c>
       <c r="J12">
-        <v>4420</v>
+        <v>4390</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="L12">
-        <v>33</v>
+        <v>1144</v>
       </c>
       <c r="M12">
         <v>30</v>
@@ -1162,7 +1170,7 @@
         <v>29</v>
       </c>
       <c r="Q12">
-        <v>3400</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1173,46 +1181,49 @@
         <v>17</v>
       </c>
       <c r="C13" s="3">
-        <v>44121</v>
+        <v>44105</v>
       </c>
       <c r="D13">
-        <v>4209</v>
+        <v>2673</v>
       </c>
       <c r="E13">
-        <v>1670</v>
+        <v>20908</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="H13">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J13">
-        <v>4580</v>
+        <v>4390</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="L13">
+        <v>222</v>
       </c>
       <c r="M13">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="N13" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="O13">
-        <v>420</v>
+        <v>340</v>
       </c>
       <c r="P13" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="Q13">
-        <v>4231</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1223,19 +1234,19 @@
         <v>17</v>
       </c>
       <c r="C14" s="3">
-        <v>44121</v>
+        <v>44105</v>
       </c>
       <c r="D14">
-        <v>4209</v>
+        <v>2200</v>
       </c>
       <c r="E14">
-        <v>1670</v>
+        <v>67179</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H14">
         <v>45</v>
@@ -1244,28 +1255,28 @@
         <v>20</v>
       </c>
       <c r="J14">
-        <v>4580</v>
+        <v>4600</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L14">
+        <v>249</v>
+      </c>
+      <c r="M14">
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14">
         <v>222</v>
       </c>
-      <c r="M14">
-        <v>41</v>
-      </c>
-      <c r="N14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14">
-        <v>420</v>
-      </c>
       <c r="P14" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="Q14">
-        <v>4231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1279,46 +1290,46 @@
         <v>44105</v>
       </c>
       <c r="D15">
-        <v>2673</v>
+        <v>2200</v>
       </c>
       <c r="E15">
-        <v>20908</v>
+        <v>67179</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H15">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J15">
-        <v>4390</v>
+        <v>4600</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L15">
-        <v>1144</v>
+        <v>12321</v>
       </c>
       <c r="M15">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O15">
-        <v>340</v>
+        <v>222</v>
       </c>
       <c r="P15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Q15">
-        <v>3421</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1329,19 +1340,19 @@
         <v>17</v>
       </c>
       <c r="C16" s="3">
-        <v>44105</v>
+        <v>44115</v>
       </c>
       <c r="D16">
-        <v>2673</v>
+        <v>3460</v>
       </c>
       <c r="E16">
-        <v>20908</v>
+        <v>76785</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H16">
         <v>43</v>
@@ -1350,28 +1361,28 @@
         <v>26</v>
       </c>
       <c r="J16">
-        <v>4390</v>
+        <v>4440</v>
       </c>
       <c r="K16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L16">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="M16">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O16">
-        <v>340</v>
+        <v>221</v>
       </c>
       <c r="P16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Q16">
-        <v>3421</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1382,34 +1393,34 @@
         <v>17</v>
       </c>
       <c r="C17" s="3">
-        <v>44105</v>
+        <v>44115</v>
       </c>
       <c r="D17">
-        <v>2200</v>
+        <v>3460</v>
       </c>
       <c r="E17">
-        <v>67179</v>
+        <v>76785</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H17">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J17">
-        <v>4600</v>
+        <v>4440</v>
       </c>
       <c r="K17" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="L17">
-        <v>249</v>
+        <v>50.4</v>
       </c>
       <c r="M17">
         <v>20</v>
@@ -1418,168 +1429,12 @@
         <v>22</v>
       </c>
       <c r="O17">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="Q17">
-        <v>2230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>405</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3">
-        <v>44105</v>
-      </c>
-      <c r="D18">
-        <v>2200</v>
-      </c>
-      <c r="E18">
-        <v>67179</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18">
-        <v>45</v>
-      </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18">
-        <v>4600</v>
-      </c>
-      <c r="K18" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18">
-        <v>12321</v>
-      </c>
-      <c r="M18">
-        <v>20</v>
-      </c>
-      <c r="N18" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18">
-        <v>222</v>
-      </c>
-      <c r="P18" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q18">
-        <v>2230</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>405</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3">
-        <v>44115</v>
-      </c>
-      <c r="D19">
-        <v>3460</v>
-      </c>
-      <c r="E19">
-        <v>76785</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19">
-        <v>43</v>
-      </c>
-      <c r="I19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19">
-        <v>4440</v>
-      </c>
-      <c r="K19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L19">
-        <v>231</v>
-      </c>
-      <c r="M19">
-        <v>20</v>
-      </c>
-      <c r="N19" t="s">
-        <v>22</v>
-      </c>
-      <c r="O19">
-        <v>221</v>
-      </c>
-      <c r="P19" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q19">
-        <v>2211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>405</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="3">
-        <v>44115</v>
-      </c>
-      <c r="D20">
-        <v>3460</v>
-      </c>
-      <c r="E20">
-        <v>76785</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20">
-        <v>43</v>
-      </c>
-      <c r="I20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20">
-        <v>4440</v>
-      </c>
-      <c r="K20" t="s">
-        <v>32</v>
-      </c>
-      <c r="L20">
-        <v>50.4</v>
-      </c>
-      <c r="M20">
-        <v>20</v>
-      </c>
-      <c r="N20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20">
-        <v>221</v>
-      </c>
-      <c r="P20" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q20">
         <v>2211</v>
       </c>
     </row>

</xml_diff>